<commit_message>
Automation Project with Cucumber framwork
</commit_message>
<xml_diff>
--- a/src/test/resources/dataRepo/FACEBOOK.xlsx
+++ b/src/test/resources/dataRepo/FACEBOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="18630" windowHeight="8595"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="18735" windowHeight="8595"/>
   </bookViews>
   <sheets>
     <sheet name="ANUSHNAREGISTRATION" sheetId="1" r:id="rId1"/>
@@ -422,7 +422,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>